<commit_message>
'correcção do bonecos apenas para IE'
</commit_message>
<xml_diff>
--- a/ficheiros/precario.xlsx
+++ b/ficheiros/precario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="52">
   <si>
     <t>Tabela Privat</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Entrada em vigor: 01 de Janeiro de 2010</t>
+  </si>
+  <si>
+    <t>Transferências para o resto do Mundo</t>
   </si>
 </sst>
 </file>
@@ -570,6 +573,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,36 +614,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1794,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1809,15 +1812,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="48" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
@@ -1830,27 +1833,27 @@
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="31"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="55" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1859,8 +1862,8 @@
         <v>37</v>
       </c>
       <c r="B5" s="40"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2264,7 +2267,7 @@
     </row>
     <row r="37" spans="1:5" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B37" s="35"/>
       <c r="C37" s="44"/>

</xml_diff>